<commit_message>
Added save function, android context needed
</commit_message>
<xml_diff>
--- a/PMSheets/PM31_01_19 .xlsx
+++ b/PMSheets/PM31_01_19 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herob\project-proposal-walliserwagner\PMSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFA11A5-46CF-4060-A589-6A664898A569}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77CCFDC-3B38-46CF-B4C6-3D4348A296B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{E0BBA045-77F2-490B-811A-0A4098F11621}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,10 +518,10 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>

</xml_diff>